<commit_message>
change port for API in configuration_delphes_jm.xlsx
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_jm.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_jm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/apps/delphes/runtime/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B961E-3D63-F144-9A9F-01F200D44B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C63740-4D44-C24D-BBF7-4D2FB1E2D46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -1282,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDFDD5-DDA9-4342-AD9F-1784F0C7F8C5}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1338,7 +1338,7 @@
         <v>144</v>
       </c>
       <c r="B5" s="13">
-        <v>8002</v>
+        <v>8052</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2495,7 +2495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>